<commit_message>
Fix Css Row in Create generator
</commit_message>
<xml_diff>
--- a/TestData/Data/Specialty.xlsx
+++ b/TestData/Data/Specialty.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fouad.Systems\Desktop\Test_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Trainning_Institution_System\1-Cplus\TestData\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -143,9 +143,6 @@
     <t>AG_INFO_TS</t>
   </si>
   <si>
-    <t>AG_INFO</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -180,6 +177,9 @@
   </si>
   <si>
     <t>Secteur</t>
+  </si>
+  <si>
+    <t>INFO</t>
   </si>
 </sst>
 </file>
@@ -517,15 +517,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.140625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="17.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="22.42578125" style="1" customWidth="1"/>
@@ -534,31 +537,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -569,16 +572,16 @@
         <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>5</v>
@@ -595,7 +598,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>38</v>

</xml_diff>